<commit_message>
completed submission of blend
</commit_message>
<xml_diff>
--- a/XTXStarterKit-dev/scores.xlsx
+++ b/XTXStarterKit-dev/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XTX Forecasting Challenge\XTXStarterKit-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2C8245-8BDF-42DB-A8B0-C93CE6E180B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281B6727-7CD7-4EB2-908E-2B45E959EAC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Didn't even fully train on training set (only used last fold in a k=5 rolling split)</t>
+  </si>
+  <si>
+    <t>lasso_drop</t>
+  </si>
+  <si>
+    <t>lasso</t>
+  </si>
+  <si>
+    <t>Henceforth, all have sigmoids</t>
+  </si>
+  <si>
+    <t>blend 4,5</t>
   </si>
 </sst>
 </file>
@@ -73,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +97,14 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,12 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,41 +512,78 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>1.8942244488987101E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>-4.0627901791395402</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>-0.51822999999999997</v>
       </c>
-      <c r="F4" s="1">
-        <f>C4-E4</f>
+      <c r="F5" s="1">
+        <f>C5-E5</f>
         <v>0.53717224448898704</v>
       </c>
-      <c r="G4" s="1">
-        <f>D4-E4</f>
+      <c r="G5" s="1">
+        <f>D5-E5</f>
         <v>-3.5445601791395402</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="1"/>
-    </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>5.0599999999999999E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-0.36285563865669301</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="1"/>
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>5.8599999999999999E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-2.06886488756439</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="1"/>
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.6668160474799401E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
@@ -547,6 +605,9 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made submissions, awaiting blend10 submission
</commit_message>
<xml_diff>
--- a/XTXStarterKit-dev/scores.xlsx
+++ b/XTXStarterKit-dev/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XTX Forecasting Challenge\XTXStarterKit-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281B6727-7CD7-4EB2-908E-2B45E959EAC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031BF23-5898-4B76-9048-B9DC7DC2D5FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -76,6 +76,27 @@
   </si>
   <si>
     <t>blend 4,5</t>
+  </si>
+  <si>
+    <t>Error: Timed out</t>
+  </si>
+  <si>
+    <t>Runs 100 in 42s, 500 in 500s</t>
+  </si>
+  <si>
+    <t>Runs 100 in 42s</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>blend 4,5 with sigmoid_drop using lasso</t>
+  </si>
+  <si>
+    <t>blend 4,5 with sigmoid_drop using lasso_drop</t>
+  </si>
+  <si>
+    <t>Awaiting submission</t>
   </si>
 </sst>
 </file>
@@ -85,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +124,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -136,13 +164,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +470,7 @@
     <col min="7" max="7" width="7.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -485,7 +516,7 @@
         <v>2.3989906542055701E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -511,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
@@ -521,7 +552,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -546,67 +577,150 @@
         <v>-3.5445601791395402</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>-0.36285563865669301</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>-2.06886488756439</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
         <v>4.6668160474799401E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5.0599999999999999E-2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>-0.36285563865669301</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.8599999999999999E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>-2.06886488756439</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7">
+        <v>-0.64641597628391601</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7">
+        <v>4.6677494892257802E-2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
they rejected all my submissions :((
</commit_message>
<xml_diff>
--- a/XTXStarterKit-dev/scores.xlsx
+++ b/XTXStarterKit-dev/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XTX Forecasting Challenge\XTXStarterKit-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031BF23-5898-4B76-9048-B9DC7DC2D5FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F29D649-6F56-4A55-9AEC-85416DC38E86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Model</t>
   </si>
@@ -90,13 +90,22 @@
     <t>Submitted</t>
   </si>
   <si>
-    <t>blend 4,5 with sigmoid_drop using lasso</t>
-  </si>
-  <si>
     <t>blend 4,5 with sigmoid_drop using lasso_drop</t>
   </si>
   <si>
     <t>Awaiting submission</t>
+  </si>
+  <si>
+    <t>Expect this to beat 8</t>
+  </si>
+  <si>
+    <t>Expect this to beat 7</t>
+  </si>
+  <si>
+    <t>lasso_minimal_14vars</t>
+  </si>
+  <si>
+    <t>Expect this to beat 9</t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +479,7 @@
     <col min="7" max="7" width="7.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -516,7 +525,7 @@
         <v>2.3989906542055701E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -542,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
@@ -552,7 +561,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -577,7 +586,7 @@
         <v>-3.5445601791395402</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -597,7 +606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -617,7 +626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -635,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -655,7 +664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -674,13 +683,16 @@
       <c r="K10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="7">
@@ -692,35 +704,39 @@
       <c r="K11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="7">
-        <v>4.6677494892257802E-2</v>
-      </c>
+      <c r="D12" s="7"/>
       <c r="K12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lgbm reaches 0.30 in batch mode
</commit_message>
<xml_diff>
--- a/XTXStarterKit-dev/scores.xlsx
+++ b/XTXStarterKit-dev/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XTX Forecasting Challenge\XTXStarterKit-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FAEC1A-22CB-4E5B-B54B-87AD1BCAC521}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A640685-98E4-47B9-BFD5-2A6809D80927}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,12 +48,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>Trial GAP</t>
-  </si>
-  <si>
     <t>CV GAP</t>
   </si>
   <si>
@@ -102,16 +96,22 @@
     <t>lasso_limited</t>
   </si>
   <si>
-    <t>Trial100</t>
-  </si>
-  <si>
-    <t>Trial500</t>
-  </si>
-  <si>
     <t>lasso_limited_nosigmoid</t>
   </si>
   <si>
     <t>lasso_limited_nosigmoid with proper cv</t>
+  </si>
+  <si>
+    <t>lgbm</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -187,7 +187,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -469,321 +468,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.296875" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="3" max="3" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.09765625" customWidth="1"/>
-    <col min="8" max="8" width="7.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1">
-        <v>2.9949906542055701E-2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.7930888575466899E-3</v>
-      </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="1">
         <v>5.96E-3</v>
       </c>
       <c r="G2" s="1">
-        <f>C2-F2</f>
+        <f>E2-F2</f>
         <v>-5.96E-3</v>
       </c>
-      <c r="H2" s="1">
-        <f>D2-F2</f>
-        <v>2.3989906542055701E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E3" s="2">
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="D3" s="3">
-        <v>-3.5112783303716499</v>
-      </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3">
-        <f>C3-F3</f>
+        <f>E3-F3</f>
         <v>1.8700000000000001E-2</v>
       </c>
-      <c r="H3" s="3">
-        <f>D3-F3</f>
-        <v>-3.5112783303716499</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
         <v>1.8942244488987101E-2</v>
       </c>
-      <c r="D5" s="1">
-        <v>-4.0627901791395402</v>
-      </c>
-      <c r="E5" s="1"/>
       <c r="F5">
         <v>-0.51822999999999997</v>
       </c>
       <c r="G5" s="1">
-        <f>C5-F5</f>
+        <f>E5-F5</f>
         <v>0.53717224448898704</v>
       </c>
-      <c r="H5" s="1">
-        <f>D5-F5</f>
-        <v>-3.5445601791395402</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="D6" s="3">
-        <v>-0.36285563865669301</v>
-      </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="D7" s="3">
-        <v>-2.06886488756439</v>
-      </c>
-      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="3">
-        <v>4.6668160474799401E-2</v>
-      </c>
-      <c r="E8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="6">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="D9" s="7">
-        <v>-0.36285563865669301</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="I9" t="s">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="D10" s="7">
-        <v>-2.06886488756439</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="I10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="7">
-        <v>-0.64641597628391601</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="I11" t="s">
         <v>16</v>
       </c>
-      <c r="L11" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
         <v>17</v>
       </c>
-      <c r="N11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13">
         <v>6.2399999999999997E-2</v>
       </c>
-      <c r="D13" s="1">
-        <v>-0.231743620211431</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6.46079210285945E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14">
         <v>6.2799999999999995E-2</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>0.19789999999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.3099999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Submit lgbm (0.0251, 0.0217, 0.0226)
</commit_message>
<xml_diff>
--- a/XTXStarterKit-dev/scores.xlsx
+++ b/XTXStarterKit-dev/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XTX Forecasting Challenge\XTXStarterKit-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F8992A-793A-4048-8078-9836942E46B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F81E645-8564-4620-A7E5-630101E7DA47}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Model</t>
   </si>
@@ -78,18 +78,9 @@
     <t>Runs 100 in 42s</t>
   </si>
   <si>
-    <t>Submitted</t>
-  </si>
-  <si>
     <t>blend 4,5 with sigmoid_drop using lasso_drop</t>
   </si>
   <si>
-    <t>Expect this to beat 8</t>
-  </si>
-  <si>
-    <t>Expect this to beat 7</t>
-  </si>
-  <si>
     <t>lasso_minimal_14vars</t>
   </si>
   <si>
@@ -115,14 +106,18 @@
   </si>
   <si>
     <t>lgbm120</t>
+  </si>
+  <si>
+    <t>lgbm 0.0226</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -182,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -191,6 +186,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,34 +467,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -510,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -526,7 +521,7 @@
         <v>-5.96E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -545,7 +540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -555,7 +550,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -573,7 +568,7 @@
         <v>0.53717224448898704</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -591,7 +586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -609,7 +604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -625,7 +620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -640,11 +635,8 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -659,19 +651,13 @@
       <c r="H10" t="s">
         <v>14</v>
       </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -679,30 +665,24 @@
       <c r="H11" t="s">
         <v>14</v>
       </c>
-      <c r="K11" t="s">
-        <v>15</v>
-      </c>
-      <c r="M11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -710,12 +690,12 @@
         <v>6.2399999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -723,39 +703,75 @@
         <v>6.2799999999999995E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16">
-        <v>0.19789999999999999</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5.5899999999999998E-2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4.3099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1.7950000000000001E-2</v>
+      </c>
+      <c r="G17" s="8">
+        <f>E17-F17</f>
+        <v>1.3500000000000005E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2.2599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>